<commit_message>
adicionado requerimentos, caso de uso. Versao inicial
</commit_message>
<xml_diff>
--- a/doc/Anteprojeto/gantt.xlsx
+++ b/doc/Anteprojeto/gantt.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
   <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F827153-987B-4536-8905-5EFCE3A646DA}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12570"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Plan1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="25">
   <si>
     <t>Atividade</t>
   </si>
@@ -98,11 +99,14 @@
   <si>
     <t>Analise sobre melhorias em VANT utilizado</t>
   </si>
+  <si>
+    <t>Levantamento dos requisitos gerais, funcionais e não funcionais do projeto</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -153,7 +157,7 @@
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="pt-BR"/>
   <c:roundedCorners val="0"/>
@@ -197,7 +201,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -313,7 +316,7 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+          <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-3275-45D8-BC61-D42EE9D7B004}"/>
             </c:ext>
@@ -400,7 +403,7 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+          <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-3275-45D8-BC61-D42EE9D7B004}"/>
             </c:ext>
@@ -538,14 +541,14 @@
     </c:plotArea>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="0"/>
-    <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+    <c:extLst>
       <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
         <c16r3:dataDisplayOptions16>
           <c16r3:dispNaAsBlank val="1"/>
         </c16r3:dataDisplayOptions16>
       </c:ext>
     </c:extLst>
+    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
     <a:solidFill>
@@ -581,7 +584,7 @@
 </file>
 
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="pt-BR"/>
   <c:roundedCorners val="0"/>
@@ -625,7 +628,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -675,43 +677,46 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Plan1!$A$12:$A$23</c:f>
+              <c:f>Plan1!$A$12:$A$24</c:f>
               <c:strCache>
-                <c:ptCount val="12"/>
+                <c:ptCount val="13"/>
                 <c:pt idx="0">
+                  <c:v>Levantamento dos requisitos gerais, funcionais e não funcionais do projeto</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>Desenho da arquitetura conceitual do sistema</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>Mapeamento das alternativas de implementação dos módulos do sistema</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>Implementação de um ambiente virtual com VANT simulado na estação de comando</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>Implementação do módulo de path planning no ambiente de virtual na estação de comando</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>Implementação do módulo de coleta de pontos e geração de trajetórias na estação de comando</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>Implementação do módulo de execução de trajetória e controle adaptativo na estação de comando</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>Analisar o funcionamento da execução de trajetórias e controle adaptativo do VANT em ambiente de simulação na estação de comando</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="8">
                   <c:v>Implementação do ambiente de simulação no VANT</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="9">
                   <c:v>Implementação da comunicação entre VANT e estação do comando</c:v>
                 </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="10">
                   <c:v>Analisar o funcionamento do controle adaptativo no ambiente de simulação no VANT</c:v>
                 </c:pt>
-                <c:pt idx="10">
+                <c:pt idx="11">
                   <c:v>Analisar o funcionamento do controle adaptativo no VANT em aplicação real</c:v>
                 </c:pt>
-                <c:pt idx="11">
+                <c:pt idx="12">
                   <c:v>Analise sobre melhorias em VANT utilizado</c:v>
                 </c:pt>
               </c:strCache>
@@ -719,50 +724,53 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Plan1!$B$12:$B$23</c:f>
+              <c:f>Plan1!$B$12:$B$24</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yyyy</c:formatCode>
-                <c:ptCount val="12"/>
+                <c:ptCount val="13"/>
                 <c:pt idx="0">
                   <c:v>43549</c:v>
                 </c:pt>
                 <c:pt idx="1">
+                  <c:v>43549</c:v>
+                </c:pt>
+                <c:pt idx="2">
                   <c:v>43552</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>43556</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>43563</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>43570</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>43577</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>43584</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="8">
                   <c:v>43556</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="9">
                   <c:v>43584</c:v>
                 </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="10">
                   <c:v>43591</c:v>
                 </c:pt>
-                <c:pt idx="10">
+                <c:pt idx="11">
                   <c:v>43598</c:v>
                 </c:pt>
-                <c:pt idx="11">
+                <c:pt idx="12">
                   <c:v>43605</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+          <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-3275-45D8-BC61-D42EE9D7B004}"/>
             </c:ext>
@@ -783,43 +791,46 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Plan1!$A$12:$A$23</c:f>
+              <c:f>Plan1!$A$12:$A$24</c:f>
               <c:strCache>
-                <c:ptCount val="12"/>
+                <c:ptCount val="13"/>
                 <c:pt idx="0">
+                  <c:v>Levantamento dos requisitos gerais, funcionais e não funcionais do projeto</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>Desenho da arquitetura conceitual do sistema</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>Mapeamento das alternativas de implementação dos módulos do sistema</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>Implementação de um ambiente virtual com VANT simulado na estação de comando</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>Implementação do módulo de path planning no ambiente de virtual na estação de comando</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>Implementação do módulo de coleta de pontos e geração de trajetórias na estação de comando</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>Implementação do módulo de execução de trajetória e controle adaptativo na estação de comando</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>Analisar o funcionamento da execução de trajetórias e controle adaptativo do VANT em ambiente de simulação na estação de comando</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="8">
                   <c:v>Implementação do ambiente de simulação no VANT</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="9">
                   <c:v>Implementação da comunicação entre VANT e estação do comando</c:v>
                 </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="10">
                   <c:v>Analisar o funcionamento do controle adaptativo no ambiente de simulação no VANT</c:v>
                 </c:pt>
-                <c:pt idx="10">
+                <c:pt idx="11">
                   <c:v>Analisar o funcionamento do controle adaptativo no VANT em aplicação real</c:v>
                 </c:pt>
-                <c:pt idx="11">
+                <c:pt idx="12">
                   <c:v>Analise sobre melhorias em VANT utilizado</c:v>
                 </c:pt>
               </c:strCache>
@@ -827,18 +838,18 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Plan1!$C$12:$C$23</c:f>
+              <c:f>Plan1!$C$12:$C$24</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="12"/>
+                <c:ptCount val="13"/>
                 <c:pt idx="0">
                   <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="1">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="2">
                   <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>7</c:v>
@@ -865,12 +876,15 @@
                   <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="11">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="12">
                   <c:v>7</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+          <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-3275-45D8-BC61-D42EE9D7B004}"/>
             </c:ext>
@@ -1007,14 +1021,14 @@
     </c:plotArea>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="0"/>
-    <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+    <c:extLst>
       <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
         <c16r3:dataDisplayOptions16>
           <c16r3:dispNaAsBlank val="1"/>
         </c16r3:dataDisplayOptions16>
       </c:ext>
     </c:extLst>
+    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
     <a:solidFill>
@@ -2159,7 +2173,7 @@
         <xdr:cNvPr id="3" name="Gráfico 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{011477C6-B437-4BD8-83B4-F3BC9719E622}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2195,7 +2209,7 @@
         <xdr:cNvPr id="6" name="Gráfico 5">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{011477C6-B437-4BD8-83B4-F3BC9719E622}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000006000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2480,21 +2494,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="N38" sqref="N38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="132.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="132.88671875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2508,7 +2522,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -2523,7 +2537,7 @@
         <v>43563</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -2539,7 +2553,7 @@
         <v>43577</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -2555,7 +2569,7 @@
         <v>43591</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>8</v>
       </c>
@@ -2571,7 +2585,7 @@
         <v>43605</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>9</v>
       </c>
@@ -2587,7 +2601,7 @@
         <v>43619</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>11</v>
       </c>
@@ -2603,7 +2617,7 @@
         <v>43626</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>10</v>
       </c>
@@ -2619,7 +2633,7 @@
         <v>43640</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>7</v>
       </c>
@@ -2635,7 +2649,7 @@
         <v>43647</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B11" t="s">
         <v>1</v>
       </c>
@@ -2646,9 +2660,9 @@
         <v>3</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="B12" s="1">
         <v>43549</v>
@@ -2661,185 +2675,196 @@
         <v>43552</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
+        <v>12</v>
+      </c>
+      <c r="B13" s="1">
+        <v>43549</v>
+      </c>
+      <c r="C13">
+        <v>3</v>
+      </c>
+      <c r="D13" s="1">
+        <f>B13+C13</f>
+        <v>43552</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
         <v>13</v>
       </c>
-      <c r="B13" s="1">
-        <f>D12</f>
+      <c r="B14" s="1">
+        <f>D13</f>
         <v>43552</v>
       </c>
-      <c r="C13">
+      <c r="C14">
         <v>4</v>
       </c>
-      <c r="D13" s="1">
-        <f t="shared" ref="D13:D22" si="2">B13+C13</f>
+      <c r="D14" s="1">
+        <f t="shared" ref="D14:D22" si="2">B14+C14</f>
         <v>43556</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
         <v>14</v>
       </c>
-      <c r="B14" s="1">
-        <f t="shared" ref="B14:B22" si="3">D13</f>
+      <c r="B15" s="1">
+        <f t="shared" ref="B15:B23" si="3">D14</f>
         <v>43556</v>
       </c>
-      <c r="C14">
+      <c r="C15">
         <v>7</v>
       </c>
-      <c r="D14" s="1">
+      <c r="D15" s="1">
         <f t="shared" si="2"/>
         <v>43563</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
         <v>15</v>
       </c>
-      <c r="B15" s="1">
+      <c r="B16" s="1">
         <f t="shared" si="3"/>
         <v>43563</v>
       </c>
-      <c r="C15">
+      <c r="C16">
         <v>7</v>
       </c>
-      <c r="D15" s="1">
+      <c r="D16" s="1">
         <f t="shared" si="2"/>
         <v>43570</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
         <v>16</v>
       </c>
-      <c r="B16" s="1">
+      <c r="B17" s="1">
         <f t="shared" si="3"/>
         <v>43570</v>
       </c>
-      <c r="C16">
+      <c r="C17">
         <v>7</v>
       </c>
-      <c r="D16" s="1">
+      <c r="D17" s="1">
         <f t="shared" si="2"/>
         <v>43577</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
         <v>17</v>
       </c>
-      <c r="B17" s="1">
+      <c r="B18" s="1">
         <f t="shared" si="3"/>
         <v>43577</v>
       </c>
-      <c r="C17">
+      <c r="C18">
         <v>7</v>
       </c>
-      <c r="D17" s="1">
+      <c r="D18" s="1">
         <f t="shared" si="2"/>
         <v>43584</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
         <v>18</v>
       </c>
-      <c r="B18" s="1">
+      <c r="B19" s="1">
         <f t="shared" si="3"/>
         <v>43584</v>
       </c>
-      <c r="C18">
+      <c r="C19">
         <v>7</v>
       </c>
-      <c r="D18" s="1">
+      <c r="D19" s="1">
         <f t="shared" si="2"/>
         <v>43591</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
         <v>19</v>
       </c>
-      <c r="B19" s="1">
-        <f>+B14</f>
+      <c r="B20" s="1">
+        <f>+B15</f>
         <v>43556</v>
       </c>
-      <c r="C19">
+      <c r="C20">
         <v>7</v>
       </c>
-      <c r="D19" s="1">
+      <c r="D20" s="1">
         <f t="shared" si="2"/>
         <v>43563</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
         <v>20</v>
       </c>
-      <c r="B20" s="1">
-        <f>+B18</f>
+      <c r="B21" s="1">
+        <f>+B19</f>
         <v>43584</v>
       </c>
-      <c r="C20">
+      <c r="C21">
         <v>7</v>
       </c>
-      <c r="D20" s="1">
+      <c r="D21" s="1">
         <f t="shared" si="2"/>
         <v>43591</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
         <v>21</v>
       </c>
-      <c r="B21" s="1">
+      <c r="B22" s="1">
         <f t="shared" si="3"/>
         <v>43591</v>
       </c>
-      <c r="C21">
+      <c r="C22">
         <v>7</v>
       </c>
-      <c r="D21" s="1">
+      <c r="D22" s="1">
         <f t="shared" si="2"/>
         <v>43598</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
         <v>22</v>
       </c>
-      <c r="B22" s="1">
+      <c r="B23" s="1">
         <f t="shared" si="3"/>
         <v>43598</v>
       </c>
-      <c r="C22">
-        <v>7</v>
-      </c>
-      <c r="D22" s="1">
-        <f>B22+C22</f>
-        <v>43605</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>23</v>
-      </c>
-      <c r="B23" s="1">
-        <f t="shared" ref="B15:B23" si="4">D22</f>
-        <v>43605</v>
-      </c>
       <c r="C23">
         <v>7</v>
       </c>
       <c r="D23" s="1">
         <f>B23+C23</f>
+        <v>43605</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>23</v>
+      </c>
+      <c r="B24" s="1">
+        <f t="shared" ref="B24" si="4">D23</f>
+        <v>43605</v>
+      </c>
+      <c r="C24">
+        <v>7</v>
+      </c>
+      <c r="D24" s="1">
+        <f>B24+C24</f>
         <v>43612</v>
       </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B24" s="1"/>
-      <c r="D24" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>